<commit_message>
First complete version of the code submitted
</commit_message>
<xml_diff>
--- a/Project_python/out/LDA/test_natureS1.xlsx
+++ b/Project_python/out/LDA/test_natureS1.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.13|x3: 0.15|x4: 0.00|x5: 0.07|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.44|x11: 0.00|x12: 0.00|x13: 0.41|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.12|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.12|x9: 0.00|x10: 0.00|x11: 0.24|x12: 0.46|x13: 0.06|x14: 0.29|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -501,12 +501,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.44]</t>
+          <t>[0.00, 0.08, 0.46]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12, 14]</t>
         </is>
       </c>
       <c r="H2" t="b">
@@ -532,7 +532,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>x1: 0.16|x2: 0.12|x3: 0.00|x4: 0.19|x5: 0.00|x6: 0.00|x7: 0.13|x8: 0.10|x9: 0.15|x10: 0.24|x11: 0.00|x12: 0.00|x13: 0.21|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.15|x2: 0.00|x3: 0.00|x4: 0.10|x5: 0.08|x6: 0.00|x7: 0.06|x8: 0.15|x9: 0.14|x10: 0.06|x11: 0.17|x12: 0.31|x13: 0.07|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -542,12 +542,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.24]</t>
+          <t>[0.00, 0.08, 0.31]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H3" t="b">
@@ -573,7 +573,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>x1: 0.09|x2: 0.00|x3: 0.07|x4: 0.11|x5: 0.00|x6: 0.06|x7: 0.14|x8: 0.00|x9: 0.08|x10: 0.20|x11: 0.12|x12: 0.08|x13: 0.24|x14: 0.00|x15: 0.12|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.20|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.06|x8: 0.11|x9: 0.12|x10: 0.00|x11: 0.21|x12: 0.27|x13: 0.06|x14: 0.12|x15: 0.08|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -583,12 +583,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.24]</t>
+          <t>[0.00, 0.08, 0.27]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H4" t="b">
@@ -614,7 +614,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>x1: 0.15|x2: 0.10|x3: 0.00|x4: 0.19|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.00|x9: 0.11|x10: 0.27|x11: 0.00|x12: 0.00|x13: 0.23|x14: 0.00|x15: 0.00|x16: 0.20|x17: 0.00</t>
+          <t>x1: 0.19|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.08|x9: 0.07|x10: 0.26|x11: 0.13|x12: 0.17|x13: 0.08|x14: 0.14|x15: 0.06|x16: 0.10|x17: 0.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,12 +624,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[10]</t>
         </is>
       </c>
       <c r="H5" t="b">
@@ -655,7 +655,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.24|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.11|x7: 0.10|x8: 0.00|x9: 0.15|x10: 0.18|x11: 0.00|x12: 0.22|x13: 0.18|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.13|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.06|x7: 0.00|x8: 0.00|x9: 0.14|x10: 0.00|x11: 0.29|x12: 0.59|x13: 0.00|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -665,19 +665,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.24]</t>
+          <t>[0.00, 0.08, 0.59]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[2, 12]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -696,7 +696,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.00|x3: 0.11|x4: 0.09|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.25|x9: 0.18|x10: 0.14|x11: 0.00|x12: 0.07|x13: 0.15|x14: 0.09|x15: 0.00|x16: 0.14|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.07|x4: 0.10|x5: 0.08|x6: 0.00|x7: 0.00|x8: 0.24|x9: 0.11|x10: 0.00|x11: 0.18|x12: 0.26|x13: 0.07|x14: 0.20|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -706,12 +706,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[8, 12]</t>
         </is>
       </c>
       <c r="H7" t="b">
@@ -737,7 +737,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.06|x3: 0.00|x4: 0.06|x5: 0.00|x6: 0.00|x7: 0.12|x8: 0.00|x9: 0.14|x10: 0.36|x11: 0.00|x12: 0.06|x13: 0.36|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.10|x2: 0.10|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.00|x9: 0.25|x10: 0.07|x11: 0.18|x12: 0.42|x13: 0.00|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -747,12 +747,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.42]</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[9, 12]</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -778,7 +778,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.00|x3: 0.00|x4: 0.09|x5: 0.09|x6: 0.10|x7: 0.11|x8: 0.07|x9: 0.00|x10: 0.23|x11: 0.11|x12: 0.07|x13: 0.35|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.14|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.06|x8: 0.15|x9: 0.00|x10: 0.09|x11: 0.27|x12: 0.28|x13: 0.24|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -788,12 +788,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.35]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12, 13]</t>
         </is>
       </c>
       <c r="H9" t="b">
@@ -819,7 +819,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.18|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.09|x8: 0.19|x9: 0.12|x10: 0.17|x11: 0.00|x12: 0.21|x13: 0.28|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.12|x9: 0.07|x10: 0.08|x11: 0.18|x12: 0.22|x13: 0.24|x14: 0.17|x15: 0.07|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.28]</t>
+          <t>[0.00, 0.08, 0.24]</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -860,7 +860,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>x1: 0.13|x2: 0.06|x3: 0.00|x4: 0.15|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.00|x9: 0.00|x10: 0.29|x11: 0.00|x12: 0.15|x13: 0.27|x14: 0.00|x15: 0.05|x16: 0.15|x17: 0.00</t>
+          <t>x1: 0.29|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.08|x8: 0.10|x9: 0.00|x10: 0.07|x11: 0.13|x12: 0.24|x13: 0.08|x14: 0.13|x15: 0.06|x16: 0.06|x17: 0.00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[1, 12]</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -901,7 +901,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.13|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.07|x9: 0.09|x10: 0.16|x11: 0.06|x12: 0.20|x13: 0.22|x14: 0.07|x15: 0.16|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.17|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.15|x10: 0.00|x11: 0.20|x12: 0.26|x13: 0.10|x14: 0.00|x15: 0.25|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -911,12 +911,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.22]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[12, 13]</t>
+          <t>[11, 12, 15]</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -942,7 +942,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>x1: 0.23|x2: 0.23|x3: 0.00|x4: 0.27|x5: 0.00|x6: 0.00|x7: 0.14|x8: 0.00|x9: 0.00|x10: 0.20|x11: 0.00|x12: 0.00|x13: 0.12|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.38|x2: 0.11|x3: 0.00|x4: 0.07|x5: 0.00|x6: 0.00|x7: 0.14|x8: 0.08|x9: 0.09|x10: 0.07|x11: 0.11|x12: 0.17|x13: 0.09|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -952,19 +952,19 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.38]</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[1, 2, 4]</t>
+          <t>[1]</t>
         </is>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -983,7 +983,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.00|x3: 0.20|x4: 0.09|x5: 0.00|x6: 0.00|x7: 0.14|x8: 0.00|x9: 0.20|x10: 0.22|x11: 0.06|x12: 0.00|x13: 0.23|x14: 0.00|x15: 0.00|x16: 0.09|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.08|x3: 0.18|x4: 0.11|x5: 0.11|x6: 0.00|x7: 0.11|x8: 0.00|x9: 0.11|x10: 0.00|x11: 0.15|x12: 0.23|x13: 0.00|x14: 0.00|x15: 0.13|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -998,7 +998,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H14" t="b">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.24|x3: 0.22|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.23|x11: 0.00|x12: 0.29|x13: 0.17|x14: 0.09|x15: 0.00|x16: 0.07|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.21|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.11|x9: 0.15|x10: 0.00|x11: 0.20|x12: 0.37|x13: 0.10|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1034,12 +1034,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.37]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[2, 3, 10, 12]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H15" t="b">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.10|x3: 0.46|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.24|x11: 0.00|x12: 0.08|x13: 0.35|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.11|x2: 0.00|x3: 0.38|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.09|x10: 0.09|x11: 0.15|x12: 0.31|x13: 0.06|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1075,12 +1075,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.46]</t>
+          <t>[0.00, 0.08, 0.38]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>x1: 0.13|x2: 0.11|x3: 0.00|x4: 0.17|x5: 0.00|x6: 0.13|x7: 0.08|x8: 0.00|x9: 0.17|x10: 0.12|x11: 0.00|x12: 0.15|x13: 0.17|x14: 0.00|x15: 0.00|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.06|x3: 0.08|x4: 0.09|x5: 0.12|x6: 0.00|x7: 0.07|x8: 0.11|x9: 0.06|x10: 0.00|x11: 0.13|x12: 0.26|x13: 0.08|x14: 0.05|x15: 0.00|x16: 0.12|x17: 0.00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1116,12 +1116,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.17]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H17" t="b">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.12|x3: 0.00|x4: 0.08|x5: 0.00|x6: 0.07|x7: 0.09|x8: 0.00|x9: 0.07|x10: 0.20|x11: 0.06|x12: 0.16|x13: 0.27|x14: 0.07|x15: 0.06|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.05|x3: 0.08|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.09|x8: 0.15|x9: 0.06|x10: 0.08|x11: 0.17|x12: 0.19|x13: 0.13|x14: 0.17|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1157,12 +1157,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.19]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.00|x3: 0.00|x4: 0.08|x5: 0.06|x6: 0.00|x7: 0.07|x8: 0.13|x9: 0.26|x10: 0.23|x11: 0.00|x12: 0.12|x13: 0.21|x14: 0.00|x15: 0.08|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.15|x9: 0.27|x10: 0.08|x11: 0.13|x12: 0.31|x13: 0.21|x14: 0.00|x15: 0.07|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1198,12 +1198,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.31]</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[9, 10, 13]</t>
+          <t>[9, 12, 13]</t>
         </is>
       </c>
       <c r="H19" t="b">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.14|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.08|x10: 0.31|x11: 0.00|x12: 0.23|x13: 0.38|x14: 0.16|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.06|x9: 0.07|x10: 0.00|x11: 0.25|x12: 0.49|x13: 0.19|x14: 0.09|x15: 0.07|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1239,19 +1239,19 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.38]</t>
+          <t>[0.00, 0.08, 0.49]</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[10, 12, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.10|x6: 0.00|x7: 0.00|x8: 0.20|x9: 0.00|x10: 0.24|x11: 0.00|x12: 0.00|x13: 0.26|x14: 0.13|x15: 0.23|x16: 0.07|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.11|x4: 0.13|x5: 0.10|x6: 0.00|x7: 0.00|x8: 0.19|x9: 0.07|x10: 0.21|x11: 0.00|x12: 0.06|x13: 0.07|x14: 0.28|x15: 0.08|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1280,12 +1280,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[8, 10, 13, 15]</t>
+          <t>[10, 14]</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>x1: 0.11|x2: 0.00|x3: 0.25|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.21|x9: 0.00|x10: 0.27|x11: 0.00|x12: 0.07|x13: 0.17|x14: 0.15|x15: 0.00|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.36|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.00|x10: 0.13|x11: 0.24|x12: 0.32|x13: 0.09|x14: 0.00|x15: 0.00|x16: 0.06|x17: 0.00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1321,12 +1321,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[3, 8, 10]</t>
+          <t>[3, 11, 12]</t>
         </is>
       </c>
       <c r="H22" t="b">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>x1: 0.10|x2: 0.07|x3: 0.00|x4: 0.10|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.12|x9: 0.06|x10: 0.28|x11: 0.00|x12: 0.07|x13: 0.34|x14: 0.09|x15: 0.00|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.19|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.28|x9: 0.14|x10: 0.00|x11: 0.08|x12: 0.19|x13: 0.09|x14: 0.17|x15: 0.15|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1362,12 +1362,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.34]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="H23" t="b">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.13|x3: 0.10|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.08|x8: 0.00|x9: 0.06|x10: 0.29|x11: 0.06|x12: 0.13|x13: 0.39|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.10|x7: 0.00|x8: 0.12|x9: 0.07|x10: 0.00|x11: 0.24|x12: 0.56|x13: 0.00|x14: 0.22|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1403,12 +1403,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.39]</t>
+          <t>[0.00, 0.08, 0.56]</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12, 14]</t>
         </is>
       </c>
       <c r="H24" t="b">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>x1: 0.10|x2: 0.00|x3: 0.00|x4: 0.06|x5: 0.00|x6: 0.24|x7: 0.00|x8: 0.10|x9: 0.18|x10: 0.26|x11: 0.00|x12: 0.00|x13: 0.29|x14: 0.00|x15: 0.00|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.18|x4: 0.00|x5: 0.00|x6: 0.11|x7: 0.00|x8: 0.07|x9: 0.18|x10: 0.06|x11: 0.15|x12: 0.36|x13: 0.00|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1444,12 +1444,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[6, 10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H25" t="b">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.14|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.16|x8: 0.13|x9: 0.10|x10: 0.15|x11: 0.07|x12: 0.11|x13: 0.10|x14: 0.17|x15: 0.00|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.08|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.13|x8: 0.21|x9: 0.10|x10: 0.00|x11: 0.22|x12: 0.24|x13: 0.11|x14: 0.06|x15: 0.00|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1485,19 +1485,19 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.17]</t>
+          <t>[0.00, 0.08, 0.24]</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[8, 11, 12]</t>
         </is>
       </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.15|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.20|x8: 0.00|x9: 0.27|x10: 0.17|x11: 0.15|x12: 0.21|x13: 0.06|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.23|x9: 0.31|x10: 0.00|x11: 0.28|x12: 0.33|x13: 0.08|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1526,19 +1526,19 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.33]</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[7, 9, 12]</t>
+          <t>[8, 9, 11, 12]</t>
         </is>
       </c>
       <c r="H27" t="b">
         <v>0</v>
       </c>
       <c r="I27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.16|x3: 0.20|x4: 0.00|x5: 0.07|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.14|x10: 0.24|x11: 0.00|x12: 0.25|x13: 0.24|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.14|x2: 0.00|x3: 0.19|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.09|x10: 0.00|x11: 0.15|x12: 0.35|x13: 0.10|x14: 0.19|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1567,12 +1567,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.35]</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>[10, 12, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H28" t="b">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>x1: 0.09|x2: 0.00|x3: 0.69|x4: 0.10|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.18|x11: 0.00|x12: 0.00|x13: 0.15|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.20|x2: 0.00|x3: 0.78|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.09|x12: 0.11|x13: 0.12|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.69]</t>
+          <t>[0.00, 0.08, 0.78]</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.06|x7: 0.21|x8: 0.32|x9: 0.36|x10: 0.00|x11: 0.06|x12: 0.00|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.15|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.09|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.33|x9: 0.23|x10: 0.06|x11: 0.13|x12: 0.16|x13: 0.08|x14: 0.10|x15: 0.00|x16: 0.13|x17: 0.00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1649,12 +1649,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.33]</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[7, 8, 9]</t>
+          <t>[8, 9]</t>
         </is>
       </c>
       <c r="H30" t="b">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.12|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.13|x7: 0.10|x8: 0.00|x9: 0.09|x10: 0.31|x11: 0.08|x12: 0.00|x13: 0.36|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.07|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.31|x12: 0.61|x13: 0.00|x14: 0.16|x15: 0.16|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1690,19 +1690,19 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.61]</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H31" t="b">
         <v>0</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>x1: 0.12|x2: 0.00|x3: 0.24|x4: 0.16|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.18|x10: 0.20|x11: 0.00|x12: 0.00|x13: 0.30|x14: 0.00|x15: 0.10|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.25|x4: 0.28|x5: 0.22|x6: 0.00|x7: 0.00|x8: 0.07|x9: 0.12|x10: 0.00|x11: 0.11|x12: 0.26|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1731,12 +1731,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.30]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[3, 13]</t>
+          <t>[3, 4, 5, 12]</t>
         </is>
       </c>
       <c r="H32" t="b">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.17|x3: 0.33|x4: 0.10|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.14|x11: 0.00|x12: 0.17|x13: 0.16|x14: 0.10|x15: 0.05|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.33|x4: 0.09|x5: 0.07|x6: 0.00|x7: 0.00|x8: 0.16|x9: 0.00|x10: 0.00|x11: 0.11|x12: 0.26|x13: 0.00|x14: 0.19|x15: 0.09|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H33" t="b">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.23|x3: 0.33|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.00|x9: 0.10|x10: 0.00|x11: 0.00|x12: 0.20|x13: 0.06|x14: 0.30|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.40|x4: 0.00|x5: 0.00|x6: 0.06|x7: 0.00|x8: 0.06|x9: 0.12|x10: 0.00|x11: 0.14|x12: 0.34|x13: 0.00|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1813,12 +1813,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.33]</t>
+          <t>[0.00, 0.08, 0.40]</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[2, 3, 14]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H34" t="b">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.00|x3: 0.45|x4: 0.00|x5: 0.07|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.00|x10: 0.23|x11: 0.00|x12: 0.10|x13: 0.21|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.10|x2: 0.00|x3: 0.40|x4: 0.10|x5: 0.08|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.08|x10: 0.00|x11: 0.11|x12: 0.21|x13: 0.00|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1854,12 +1854,12 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.45]</t>
+          <t>[0.00, 0.08, 0.40]</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H35" t="b">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>x1: 0.11|x2: 0.07|x3: 0.19|x4: 0.13|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.08|x10: 0.21|x11: 0.00|x12: 0.11|x13: 0.24|x14: 0.00|x15: 0.00|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.34|x2: 0.00|x3: 0.20|x4: 0.06|x5: 0.06|x6: 0.00|x7: 0.00|x8: 0.16|x9: 0.07|x10: 0.08|x11: 0.12|x12: 0.22|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1895,12 +1895,12 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.24]</t>
+          <t>[0.00, 0.08, 0.34]</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[1, 12]</t>
         </is>
       </c>
       <c r="H36" t="b">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.15|x3: 0.08|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.00|x9: 0.06|x10: 0.17|x11: 0.00|x12: 0.37|x13: 0.14|x14: 0.10|x15: 0.00|x16: 0.10|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.07|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.07|x10: 0.00|x11: 0.20|x12: 0.45|x13: 0.07|x14: 0.09|x15: 0.07|x16: 0.09|x17: 0.00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.37]</t>
+          <t>[0.00, 0.08, 0.45]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.36|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.08|x8: 0.00|x9: 0.05|x10: 0.27|x11: 0.08|x12: 0.10|x13: 0.29|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.40|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.06|x11: 0.13|x12: 0.12|x13: 0.09|x14: 0.36|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1977,12 +1977,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.40]</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[3, 14]</t>
         </is>
       </c>
       <c r="H38" t="b">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>x1: 0.12|x2: 0.00|x3: 0.38|x4: 0.16|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.21|x10: 0.14|x11: 0.00|x12: 0.12|x13: 0.16|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.35|x4: 0.00|x5: 0.00|x6: 0.07|x7: 0.00|x8: 0.00|x9: 0.14|x10: 0.00|x11: 0.14|x12: 0.32|x13: 0.07|x14: 0.15|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2018,12 +2018,12 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.38]</t>
+          <t>[0.00, 0.08, 0.35]</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[3, 9]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H39" t="b">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.11|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.05|x7: 0.18|x8: 0.00|x9: 0.28|x10: 0.11|x11: 0.10|x12: 0.23|x13: 0.13|x14: 0.00|x15: 0.00|x16: 0.10|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.07|x7: 0.08|x8: 0.11|x9: 0.07|x10: 0.00|x11: 0.20|x12: 0.32|x13: 0.09|x14: 0.16|x15: 0.06|x16: 0.14|x17: 0.00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2059,12 +2059,12 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.28]</t>
+          <t>[0.00, 0.08, 0.32]</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>[9, 12]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H40" t="b">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.27|x4: 0.00|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.10|x10: 0.28|x11: 0.00|x12: 0.09|x13: 0.26|x14: 0.13|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.15|x2: 0.00|x3: 0.24|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.11|x10: 0.00|x11: 0.20|x12: 0.37|x13: 0.06|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2100,12 +2100,12 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.28]</t>
+          <t>[0.00, 0.08, 0.37]</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H41" t="b">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.12|x3: 0.17|x4: 0.06|x5: 0.07|x6: 0.00|x7: 0.09|x8: 0.00|x9: 0.00|x10: 0.19|x11: 0.00|x12: 0.18|x13: 0.29|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.20|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.12|x9: 0.07|x10: 0.00|x11: 0.15|x12: 0.31|x13: 0.10|x14: 0.19|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2141,19 +2141,19 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.31]</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>x1: 0.09|x2: 0.00|x3: 0.36|x4: 0.10|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.12|x10: 0.19|x11: 0.00|x12: 0.08|x13: 0.18|x14: 0.18|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.35|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.18|x12: 0.37|x13: 0.06|x14: 0.19|x15: 0.09|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2182,12 +2182,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.37]</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H43" t="b">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.14|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.13|x8: 0.11|x9: 0.15|x10: 0.26|x11: 0.13|x12: 0.14|x13: 0.18|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.30|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.17|x10: 0.13|x11: 0.20|x12: 0.19|x13: 0.21|x14: 0.00|x15: 0.10|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2223,19 +2223,19 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.30]</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>[10]</t>
+          <t>[3, 13]</t>
         </is>
       </c>
       <c r="H44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.11|x3: 0.00|x4: 0.07|x5: 0.09|x6: 0.00|x7: 0.11|x8: 0.19|x9: 0.12|x10: 0.12|x11: 0.08|x12: 0.27|x13: 0.14|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.10|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.08|x6: 0.00|x7: 0.00|x8: 0.20|x9: 0.08|x10: 0.08|x11: 0.13|x12: 0.23|x13: 0.08|x14: 0.21|x15: 0.00|x16: 0.11|x17: 0.00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2264,12 +2264,12 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.23]</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[12]</t>
+          <t>[8, 12, 14]</t>
         </is>
       </c>
       <c r="H45" t="b">
@@ -2295,7 +2295,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.11|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.25|x11: 0.00|x12: 0.17|x13: 0.49|x14: 0.17|x15: 0.11|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.11|x2: 0.00|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.09|x10: 0.13|x11: 0.18|x12: 0.27|x13: 0.13|x14: 0.18|x15: 0.13|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2305,12 +2305,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.49]</t>
+          <t>[0.00, 0.08, 0.27]</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H46" t="b">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.06|x3: 0.25|x4: 0.08|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.00|x9: 0.07|x10: 0.27|x11: 0.00|x12: 0.00|x13: 0.24|x14: 0.17|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.11|x2: 0.00|x3: 0.17|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.22|x10: 0.06|x11: 0.17|x12: 0.26|x13: 0.06|x14: 0.15|x15: 0.00|x16: 0.11|x17: 0.00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2346,19 +2346,19 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[9, 12]</t>
         </is>
       </c>
       <c r="H47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>x1: 0.09|x2: 0.17|x3: 0.08|x4: 0.11|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.22|x11: 0.00|x12: 0.26|x13: 0.22|x14: 0.00|x15: 0.16|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.24|x2: 0.00|x3: 0.17|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.08|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.23|x12: 0.30|x13: 0.12|x14: 0.16|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2387,19 +2387,19 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.30]</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>[10, 12, 13]</t>
+          <t>[1, 11, 12]</t>
         </is>
       </c>
       <c r="H48" t="b">
         <v>0</v>
       </c>
       <c r="I48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>x1: 0.14|x2: 0.15|x3: 0.22|x4: 0.15|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.18|x11: 0.00|x12: 0.15|x13: 0.16|x14: 0.09|x15: 0.06|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.27|x4: 0.09|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.12|x9: 0.00|x10: 0.00|x11: 0.09|x12: 0.21|x13: 0.00|x14: 0.28|x15: 0.08|x16: 0.06|x17: 0.00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2428,12 +2428,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.22]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 12, 14]</t>
         </is>
       </c>
       <c r="H49" t="b">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>x1: 0.11|x2: 0.10|x3: 0.00|x4: 0.15|x5: 0.12|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.07|x10: 0.31|x11: 0.00|x12: 0.15|x13: 0.28|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.14|x2: 0.00|x3: 0.00|x4: 0.19|x5: 0.16|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.12|x10: 0.00|x11: 0.13|x12: 0.30|x13: 0.08|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2469,12 +2469,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.30]</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H50" t="b">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>x1: 0.10|x2: 0.10|x3: 0.09|x4: 0.12|x5: 0.10|x6: 0.00|x7: 0.00|x8: 0.16|x9: 0.07|x10: 0.19|x11: 0.00|x12: 0.11|x13: 0.18|x14: 0.00|x15: 0.06|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.19|x2: 0.00|x3: 0.11|x4: 0.11|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.09|x10: 0.00|x11: 0.12|x12: 0.29|x13: 0.00|x14: 0.06|x15: 0.14|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2510,12 +2510,12 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.19]</t>
+          <t>[0.00, 0.08, 0.29]</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H51" t="b">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>x1: 0.22|x2: 0.10|x3: 0.00|x4: 0.29|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.14|x10: 0.23|x11: 0.00|x12: 0.00|x13: 0.21|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.27|x5: 0.21|x6: 0.00|x7: 0.00|x8: 0.07|x9: 0.09|x10: 0.00|x11: 0.19|x12: 0.29|x13: 0.10|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>[1, 4, 10, 13]</t>
+          <t>[4, 5, 12]</t>
         </is>
       </c>
       <c r="H52" t="b">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>x1: 0.17|x2: 0.00|x3: 0.10|x4: 0.23|x5: 0.19|x6: 0.00|x7: 0.00|x8: 0.13|x9: 0.00|x10: 0.12|x11: 0.00|x12: 0.13|x13: 0.10|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.13|x2: 0.00|x3: 0.07|x4: 0.15|x5: 0.18|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.13|x12: 0.30|x13: 0.06|x14: 0.10|x15: 0.00|x16: 0.18|x17: 0.00</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2592,19 +2592,19 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.23]</t>
+          <t>[0.00, 0.08, 0.30]</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>x1: 0.13|x2: 0.11|x3: 0.16|x4: 0.17|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.24|x11: 0.00|x12: 0.23|x13: 0.25|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.14|x4: 0.14|x5: 0.12|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.11|x11: 0.16|x12: 0.38|x13: 0.00|x14: 0.12|x15: 0.07|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2633,12 +2633,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.38]</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>[10, 12, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H54" t="b">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>x1: 0.14|x2: 0.07|x3: 0.00|x4: 0.19|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.33|x11: 0.00|x12: 0.07|x13: 0.41|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.21|x5: 0.16|x6: 0.00|x7: 0.00|x8: 0.07|x9: 0.10|x10: 0.00|x11: 0.25|x12: 0.39|x13: 0.07|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2674,19 +2674,19 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.41]</t>
+          <t>[0.00, 0.08, 0.39]</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[4, 11, 12]</t>
         </is>
       </c>
       <c r="H55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>x1: 0.16|x2: 0.17|x3: 0.00|x4: 0.20|x5: 0.16|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.18|x11: 0.00|x12: 0.11|x13: 0.19|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.17|x2: 0.00|x3: 0.00|x4: 0.19|x5: 0.17|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.06|x10: 0.00|x11: 0.15|x12: 0.30|x13: 0.09|x14: 0.11|x15: 0.00|x16: 0.06|x17: 0.00</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2715,19 +2715,19 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.20]</t>
+          <t>[0.00, 0.08, 0.30]</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2746,7 +2746,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.06|x5: 0.15|x6: 0.00|x7: 0.00|x8: 0.21|x9: 0.09|x10: 0.41|x11: 0.00|x12: 0.00|x13: 0.37|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.07|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.35|x9: 0.16|x10: 0.15|x11: 0.17|x12: 0.40|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2756,12 +2756,12 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.41]</t>
+          <t>[0.00, 0.08, 0.40]</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>[8, 10, 13]</t>
+          <t>[8, 12]</t>
         </is>
       </c>
       <c r="H57" t="b">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>x1: 0.19|x2: 0.16|x3: 0.00|x4: 0.25|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.15|x11: 0.00|x12: 0.27|x13: 0.12|x14: 0.16|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.18|x2: 0.00|x3: 0.00|x4: 0.18|x5: 0.13|x6: 0.07|x7: 0.00|x8: 0.00|x9: 0.07|x10: 0.00|x11: 0.16|x12: 0.36|x13: 0.00|x14: 0.15|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2797,19 +2797,19 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>[4, 12]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.10|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.17|x8: 0.00|x9: 0.14|x10: 0.25|x11: 0.10|x12: 0.00|x13: 0.35|x14: 0.00|x15: 0.13|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.16|x9: 0.14|x10: 0.00|x11: 0.27|x12: 0.36|x13: 0.20|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2838,12 +2838,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.35]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H59" t="b">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.08|x3: 0.00|x4: 0.06|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.14|x9: 0.10|x10: 0.37|x11: 0.00|x12: 0.12|x13: 0.36|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.00|x4: 0.06|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.17|x9: 0.05|x10: 0.07|x11: 0.18|x12: 0.41|x13: 0.09|x14: 0.19|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2879,12 +2879,12 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.37]</t>
+          <t>[0.00, 0.08, 0.41]</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H60" t="b">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.10|x3: 0.00|x4: 0.00|x5: 0.07|x6: 0.18|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.10|x11: 0.00|x12: 0.00|x13: 0.13|x14: 0.22|x15: 0.00|x16: 0.49|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.18|x6: 0.14|x7: 0.06|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.11|x12: 0.19|x13: 0.00|x14: 0.24|x15: 0.00|x16: 0.38|x17: 0.00</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.49]</t>
+          <t>[0.00, 0.08, 0.38]</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.15|x6: 0.08|x7: 0.00|x8: 0.10|x9: 0.00|x10: 0.17|x11: 0.00|x12: 0.12|x13: 0.26|x14: 0.24|x15: 0.00|x16: 0.18|x17: 0.00</t>
+          <t>x1: 0.05|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.19|x9: 0.00|x10: 0.00|x11: 0.14|x12: 0.32|x13: 0.07|x14: 0.18|x15: 0.00|x16: 0.26|x17: 0.00</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2961,12 +2961,12 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.32]</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>[13, 14]</t>
+          <t>[12, 16]</t>
         </is>
       </c>
       <c r="H62" t="b">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.16|x3: 0.10|x4: 0.10|x5: 0.13|x6: 0.00|x7: 0.10|x8: 0.13|x9: 0.07|x10: 0.08|x11: 0.08|x12: 0.11|x13: 0.08|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.24|x2: 0.00|x3: 0.09|x4: 0.07|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.07|x9: 0.06|x10: 0.00|x11: 0.20|x12: 0.22|x13: 0.08|x14: 0.23|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -3002,12 +3002,12 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.16]</t>
+          <t>[0.00, 0.08, 0.24]</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[1, 12, 14]</t>
         </is>
       </c>
       <c r="H63" t="b">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.38|x6: 0.00|x7: 0.12|x8: 0.17|x9: 0.00|x10: 0.18|x11: 0.10|x12: 0.09|x13: 0.19|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.26|x2: 0.00|x3: 0.00|x4: 0.20|x5: 0.16|x6: 0.00|x7: 0.00|x8: 0.11|x9: 0.07|x10: 0.00|x11: 0.14|x12: 0.25|x13: 0.00|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -3043,19 +3043,19 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.38]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>[5]</t>
+          <t>[1, 12]</t>
         </is>
       </c>
       <c r="H64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -3074,7 +3074,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.08|x3: 0.00|x4: 0.00|x5: 0.29|x6: 0.00|x7: 0.08|x8: 0.10|x9: 0.13|x10: 0.19|x11: 0.00|x12: 0.10|x13: 0.25|x14: 0.00|x15: 0.00|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.12|x5: 0.15|x6: 0.07|x7: 0.00|x8: 0.12|x9: 0.07|x10: 0.00|x11: 0.10|x12: 0.24|x13: 0.05|x14: 0.21|x15: 0.00|x16: 0.17|x17: 0.00</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3084,19 +3084,19 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.24]</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>[5, 13]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -3115,7 +3115,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.00|x9: 0.25|x10: 0.43|x11: 0.07|x12: 0.00|x13: 0.32|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.08|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.11|x9: 0.28|x10: 0.07|x11: 0.20|x12: 0.38|x13: 0.18|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3125,12 +3125,12 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.43]</t>
+          <t>[0.00, 0.08, 0.38]</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>[9, 10, 13]</t>
+          <t>[9, 11, 12]</t>
         </is>
       </c>
       <c r="H66" t="b">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>x1: 0.11|x2: 0.07|x3: 0.20|x4: 0.08|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.08|x9: 0.09|x10: 0.25|x11: 0.00|x12: 0.13|x13: 0.23|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.18|x4: 0.07|x5: 0.08|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.12|x10: 0.00|x11: 0.15|x12: 0.33|x13: 0.00|x14: 0.11|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3166,12 +3166,12 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.33]</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H67" t="b">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.16|x8: 0.00|x9: 0.06|x10: 0.18|x11: 0.16|x12: 0.12|x13: 0.17|x14: 0.00|x15: 0.36|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.14|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.15|x9: 0.00|x10: 0.00|x11: 0.18|x12: 0.26|x13: 0.00|x14: 0.23|x15: 0.26|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3207,12 +3207,12 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[12, 14, 15]</t>
         </is>
       </c>
       <c r="H68" t="b">
@@ -3238,7 +3238,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>x1: 0.10|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.28|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.40|x11: 0.00|x12: 0.16|x13: 0.37|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.13|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.13|x7: 0.00|x8: 0.12|x9: 0.00|x10: 0.00|x11: 0.17|x12: 0.35|x13: 0.15|x14: 0.18|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3248,19 +3248,19 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.40]</t>
+          <t>[0.00, 0.08, 0.35]</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>[6, 10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.12|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.18|x7: 0.07|x8: 0.00|x9: 0.17|x10: 0.22|x11: 0.00|x12: 0.09|x13: 0.26|x14: 0.00|x15: 0.19|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.14|x7: 0.05|x8: 0.00|x9: 0.09|x10: 0.11|x11: 0.12|x12: 0.29|x13: 0.00|x14: 0.22|x15: 0.16|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3289,12 +3289,12 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.29]</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H70" t="b">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.11|x6: 0.00|x7: 0.10|x8: 0.11|x9: 0.00|x10: 0.29|x11: 0.09|x12: 0.08|x13: 0.34|x14: 0.00|x15: 0.18|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.08|x8: 0.13|x9: 0.15|x10: 0.00|x11: 0.22|x12: 0.34|x13: 0.15|x14: 0.07|x15: 0.10|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3335,7 +3335,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H71" t="b">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.33|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.32|x11: 0.00|x12: 0.11|x13: 0.41|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.21|x7: 0.00|x8: 0.08|x9: 0.00|x10: 0.00|x11: 0.23|x12: 0.44|x13: 0.06|x14: 0.15|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3371,12 +3371,12 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.41]</t>
+          <t>[0.00, 0.08, 0.44]</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>[6, 10, 13]</t>
+          <t>[6, 11, 12]</t>
         </is>
       </c>
       <c r="H72" t="b">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.11|x3: 0.00|x4: 0.06|x5: 0.26|x6: 0.00|x7: 0.00|x8: 0.18|x9: 0.00|x10: 0.21|x11: 0.00|x12: 0.11|x13: 0.25|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.10|x9: 0.00|x10: 0.28|x11: 0.19|x12: 0.33|x13: 0.00|x14: 0.11|x15: 0.00|x16: 0.10|x17: 0.00</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3412,12 +3412,12 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.33]</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>[5, 10, 13]</t>
+          <t>[10, 12]</t>
         </is>
       </c>
       <c r="H73" t="b">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.10|x3: 0.00|x4: 0.07|x5: 0.00|x6: 0.00|x7: 0.13|x8: 0.18|x9: 0.12|x10: 0.18|x11: 0.10|x12: 0.00|x13: 0.18|x14: 0.18|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.16|x2: 0.00|x3: 0.00|x4: 0.10|x5: 0.07|x6: 0.00|x7: 0.00|x8: 0.19|x9: 0.19|x10: 0.14|x11: 0.15|x12: 0.22|x13: 0.07|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -3453,12 +3453,12 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.18]</t>
+          <t>[0.00, 0.08, 0.22]</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H74" t="b">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.20|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.10|x7: 0.15|x8: 0.14|x9: 0.00|x10: 0.16|x11: 0.00|x12: 0.16|x13: 0.19|x14: 0.00|x15: 0.20|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.45|x9: 0.16|x10: 0.00|x11: 0.13|x12: 0.31|x13: 0.11|x14: 0.00|x15: 0.00|x16: 0.15|x17: 0.00</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3494,19 +3494,19 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.20]</t>
+          <t>[0.00, 0.08, 0.45]</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[8, 12]</t>
         </is>
       </c>
       <c r="H75" t="b">
         <v>0</v>
       </c>
       <c r="I75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>x1: 0.12|x2: 0.13|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.38|x11: 0.00|x12: 0.15|x13: 0.43|x14: 0.00|x15: 0.00|x16: 0.09|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.07|x9: 0.09|x10: 0.06|x11: 0.21|x12: 0.49|x13: 0.00|x14: 0.13|x15: 0.00|x16: 0.13|x17: 0.00</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3535,12 +3535,12 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.43]</t>
+          <t>[0.00, 0.08, 0.49]</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H76" t="b">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.00|x3: 0.13|x4: 0.09|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.39|x9: 0.00|x10: 0.23|x11: 0.06|x12: 0.00|x13: 0.26|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.12|x5: 0.09|x6: 0.00|x7: 0.06|x8: 0.31|x9: 0.10|x10: 0.00|x11: 0.22|x12: 0.16|x13: 0.13|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -3576,12 +3576,12 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.39]</t>
+          <t>[0.00, 0.08, 0.31]</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>[8, 10, 13]</t>
+          <t>[8, 11]</t>
         </is>
       </c>
       <c r="H77" t="b">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.23|x9: 0.20|x10: 0.34|x11: 0.00|x12: 0.00|x13: 0.39|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.20|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.10|x9: 0.00|x10: 0.22|x11: 0.18|x12: 0.41|x13: 0.00|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3617,12 +3617,12 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.39]</t>
+          <t>[0.00, 0.08, 0.41]</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>[8, 10, 13]</t>
+          <t>[10, 12]</t>
         </is>
       </c>
       <c r="H78" t="b">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.20|x3: 0.07|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.11|x8: 0.00|x9: 0.00|x10: 0.24|x11: 0.07|x12: 0.17|x13: 0.27|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.14|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.10|x9: 0.00|x10: 0.08|x11: 0.30|x12: 0.43|x13: 0.09|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -3658,12 +3658,12 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>[2, 10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H79" t="b">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.07|x6: 0.00|x7: 0.24|x8: 0.00|x9: 0.28|x10: 0.20|x11: 0.16|x12: 0.06|x13: 0.23|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.13|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.18|x8: 0.19|x9: 0.06|x10: 0.14|x11: 0.21|x12: 0.22|x13: 0.17|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -3699,19 +3699,19 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.28]</t>
+          <t>[0.00, 0.08, 0.22]</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>[7, 9, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3730,7 +3730,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>x1: 0.11|x2: 0.00|x3: 0.00|x4: 0.09|x5: 0.00|x6: 0.00|x7: 0.13|x8: 0.00|x9: 0.00|x10: 0.31|x11: 0.14|x12: 0.15|x13: 0.36|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.11|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.17|x9: 0.14|x10: 0.06|x11: 0.26|x12: 0.30|x13: 0.18|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3740,19 +3740,19 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.30]</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H81" t="b">
         <v>0</v>
       </c>
       <c r="I81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.09|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.41|x7: 0.06|x8: 0.00|x9: 0.00|x10: 0.21|x11: 0.07|x12: 0.16|x13: 0.20|x14: 0.00|x15: 0.00|x16: 0.10|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.06|x6: 0.25|x7: 0.00|x8: 0.10|x9: 0.07|x10: 0.00|x11: 0.22|x12: 0.39|x13: 0.08|x14: 0.13|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -3781,19 +3781,19 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.41]</t>
+          <t>[0.00, 0.08, 0.39]</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>[6, 10]</t>
+          <t>[6, 11, 12]</t>
         </is>
       </c>
       <c r="H82" t="b">
         <v>0</v>
       </c>
       <c r="I82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -3812,7 +3812,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.00|x9: 0.28|x10: 0.33|x11: 0.00|x12: 0.11|x13: 0.41|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.17|x9: 0.21|x10: 0.00|x11: 0.23|x12: 0.51|x13: 0.00|x14: 0.18|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -3822,16 +3822,16 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.41]</t>
+          <t>[0.00, 0.08, 0.51]</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>[9, 10, 13]</t>
+          <t>[9, 11, 12]</t>
         </is>
       </c>
       <c r="H83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="b">
         <v>1</v>
@@ -3853,7 +3853,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.13|x3: 0.00|x4: 0.00|x5: 0.09|x6: 0.15|x7: 0.15|x8: 0.12|x9: 0.13|x10: 0.19|x11: 0.06|x12: 0.00|x13: 0.27|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.16|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.14|x7: 0.00|x8: 0.22|x9: 0.25|x10: 0.00|x11: 0.07|x12: 0.16|x13: 0.09|x14: 0.21|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -3863,12 +3863,12 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.25]</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[8, 9, 14]</t>
         </is>
       </c>
       <c r="H84" t="b">
@@ -3894,7 +3894,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>x1: 0.11|x2: 0.08|x3: 0.12|x4: 0.14|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.10|x9: 0.00|x10: 0.22|x11: 0.00|x12: 0.06|x13: 0.25|x14: 0.07|x15: 0.00|x16: 0.07|x17: 0.00</t>
+          <t>x1: 0.11|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.07|x6: 0.00|x7: 0.06|x8: 0.18|x9: 0.00|x10: 0.06|x11: 0.14|x12: 0.33|x13: 0.00|x14: 0.08|x15: 0.00|x16: 0.20|x17: 0.00</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -3904,19 +3904,19 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.33]</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H85" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3935,7 +3935,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>x1: 0.11|x2: 0.09|x3: 0.00|x4: 0.06|x5: 0.10|x6: 0.00|x7: 0.00|x8: 0.11|x9: 0.00|x10: 0.33|x11: 0.00|x12: 0.10|x13: 0.26|x14: 0.00|x15: 0.00|x16: 0.15|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.00|x4: 0.09|x5: 0.10|x6: 0.00|x7: 0.00|x8: 0.13|x9: 0.08|x10: 0.06|x11: 0.19|x12: 0.33|x13: 0.06|x14: 0.09|x15: 0.00|x16: 0.09|x17: 0.00</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3950,14 +3950,14 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H86" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -3976,7 +3976,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.09|x3: 0.00|x4: 0.00|x5: 0.20|x6: 0.00|x7: 0.11|x8: 0.21|x9: 0.09|x10: 0.22|x11: 0.08|x12: 0.00|x13: 0.23|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.11|x5: 0.12|x6: 0.00|x7: 0.00|x8: 0.20|x9: 0.12|x10: 0.06|x11: 0.20|x12: 0.20|x13: 0.12|x14: 0.08|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3986,19 +3986,19 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.23]</t>
+          <t>[0.00, 0.08, 0.20]</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>[5, 8, 10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.12|x3: 0.07|x4: 0.11|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.00|x9: 0.00|x10: 0.22|x11: 0.07|x12: 0.21|x13: 0.25|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.26|x2: 0.00|x3: 0.05|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.09|x9: 0.07|x10: 0.00|x11: 0.21|x12: 0.33|x13: 0.07|x14: 0.09|x15: 0.07|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -4027,19 +4027,19 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.33]</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>[10, 12, 13]</t>
+          <t>[1, 11, 12]</t>
         </is>
       </c>
       <c r="H88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.10|x3: 0.00|x4: 0.08|x5: 0.10|x6: 0.00|x7: 0.06|x8: 0.14|x9: 0.10|x10: 0.19|x11: 0.00|x12: 0.09|x13: 0.31|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.10|x2: 0.00|x3: 0.00|x4: 0.07|x5: 0.06|x6: 0.10|x7: 0.00|x8: 0.24|x9: 0.00|x10: 0.00|x11: 0.16|x12: 0.24|x13: 0.24|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -4068,12 +4068,12 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.24]</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[8, 12, 13]</t>
         </is>
       </c>
       <c r="H89" t="b">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.15|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.27|x8: 0.10|x9: 0.00|x10: 0.25|x11: 0.24|x12: 0.00|x13: 0.30|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.15|x8: 0.09|x9: 0.06|x10: 0.09|x11: 0.38|x12: 0.18|x13: 0.22|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -4109,12 +4109,12 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.30]</t>
+          <t>[0.00, 0.08, 0.38]</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>[7, 10, 11, 13]</t>
+          <t>[11, 13]</t>
         </is>
       </c>
       <c r="H90" t="b">
@@ -4140,7 +4140,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.16|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.26|x8: 0.00|x9: 0.12|x10: 0.13|x11: 0.25|x12: 0.00|x13: 0.18|x14: 0.14|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.12|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.45|x12: 0.52|x13: 0.15|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -4150,12 +4150,12 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.52]</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>[7, 11]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H91" t="b">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.09|x3: 0.00|x4: 0.00|x5: 0.11|x6: 0.18|x7: 0.08|x8: 0.07|x9: 0.14|x10: 0.19|x11: 0.00|x12: 0.16|x13: 0.28|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.05|x2: 0.13|x3: 0.00|x4: 0.07|x5: 0.08|x6: 0.00|x7: 0.15|x8: 0.14|x9: 0.25|x10: 0.00|x11: 0.09|x12: 0.21|x13: 0.00|x14: 0.06|x15: 0.00|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -4191,12 +4191,12 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.28]</t>
+          <t>[0.00, 0.08, 0.25]</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[9, 12]</t>
         </is>
       </c>
       <c r="H92" t="b">
@@ -4222,7 +4222,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.14|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.13|x9: 0.18|x10: 0.30|x11: 0.00|x12: 0.00|x13: 0.36|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.09|x8: 0.19|x9: 0.22|x10: 0.00|x11: 0.29|x12: 0.36|x13: 0.10|x14: 0.00|x15: 0.06|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -4237,14 +4237,14 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[9, 11, 12]</t>
         </is>
       </c>
       <c r="H93" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.12|x3: 0.17|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.08|x9: 0.00|x10: 0.26|x11: 0.06|x12: 0.11|x13: 0.31|x14: 0.00|x15: 0.00|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.00|x3: 0.17|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.12|x10: 0.00|x11: 0.29|x12: 0.43|x13: 0.12|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -4273,19 +4273,19 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.16|x4: 0.00|x5: 0.00|x6: 0.11|x7: 0.18|x8: 0.00|x9: 0.27|x10: 0.10|x11: 0.12|x12: 0.00|x13: 0.17|x14: 0.07|x15: 0.00|x16: 0.07|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.13|x4: 0.00|x5: 0.00|x6: 0.07|x7: 0.11|x8: 0.00|x9: 0.18|x10: 0.07|x11: 0.20|x12: 0.00|x13: 0.21|x14: 0.21|x15: 0.00|x16: 0.11|x17: 0.00</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -4314,19 +4314,19 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.21]</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[11, 13, 14]</t>
         </is>
       </c>
       <c r="H95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>x1: 0.10|x2: 0.09|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.09|x8: 0.00|x9: 0.08|x10: 0.30|x11: 0.00|x12: 0.08|x13: 0.23|x14: 0.15|x15: 0.00|x16: 0.10|x17: 0.00</t>
+          <t>x1: 0.22|x2: 0.00|x3: 0.08|x4: 0.00|x5: 0.00|x6: 0.13|x7: 0.00|x8: 0.00|x9: 0.09|x10: 0.16|x11: 0.19|x12: 0.30|x13: 0.00|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[1, 12]</t>
         </is>
       </c>
       <c r="H96" t="b">
@@ -4386,7 +4386,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>x1: 0.10|x2: 0.11|x3: 0.00|x4: 0.10|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.17|x11: 0.00|x12: 0.25|x13: 0.16|x14: 0.00|x15: 0.40|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.09|x9: 0.00|x10: 0.00|x11: 0.25|x12: 0.42|x13: 0.06|x14: 0.06|x15: 0.30|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -4396,19 +4396,19 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.40]</t>
+          <t>[0.00, 0.08, 0.42]</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>[12, 15]</t>
+          <t>[11, 12, 15]</t>
         </is>
       </c>
       <c r="H97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -4427,7 +4427,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.09|x3: 0.19|x4: 0.11|x5: 0.14|x6: 0.00|x7: 0.00|x8: 0.22|x9: 0.00|x10: 0.13|x11: 0.00|x12: 0.19|x13: 0.15|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.13|x2: 0.00|x3: 0.19|x4: 0.06|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.26|x9: 0.12|x10: 0.00|x11: 0.14|x12: 0.32|x13: 0.00|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -4437,12 +4437,12 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.22]</t>
+          <t>[0.00, 0.08, 0.32]</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[8, 12]</t>
         </is>
       </c>
       <c r="H98" t="b">
@@ -4468,7 +4468,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.08|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.12|x7: 0.06|x8: 0.06|x9: 0.00|x10: 0.29|x11: 0.07|x12: 0.11|x13: 0.29|x14: 0.09|x15: 0.00|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.12|x9: 0.00|x10: 0.19|x11: 0.24|x12: 0.42|x13: 0.07|x14: 0.14|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -4478,19 +4478,19 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.42]</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H99" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.15|x3: 0.10|x4: 0.06|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.10|x9: 0.00|x10: 0.17|x11: 0.10|x12: 0.19|x13: 0.19|x14: 0.07|x15: 0.00|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.11|x4: 0.00|x5: 0.07|x6: 0.11|x7: 0.00|x8: 0.08|x9: 0.00|x10: 0.00|x11: 0.26|x12: 0.39|x13: 0.06|x14: 0.22|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -4519,19 +4519,19 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.19]</t>
+          <t>[0.00, 0.08, 0.39]</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[11, 12, 14]</t>
         </is>
       </c>
       <c r="H100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -4550,7 +4550,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.00|x9: 0.33|x10: 0.23|x11: 0.00|x12: 0.20|x13: 0.37|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.45|x10: 0.00|x11: 0.20|x12: 0.43|x13: 0.08|x14: 0.05|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -4560,12 +4560,12 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.37]</t>
+          <t>[0.00, 0.08, 0.45]</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>[9, 10, 12, 13]</t>
+          <t>[9, 12]</t>
         </is>
       </c>
       <c r="H101" t="b">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.18|x8: 0.00|x9: 0.21|x10: 0.21|x11: 0.11|x12: 0.10|x13: 0.41|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.08|x8: 0.10|x9: 0.26|x10: 0.00|x11: 0.22|x12: 0.21|x13: 0.31|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -4601,12 +4601,12 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.41]</t>
+          <t>[0.00, 0.08, 0.31]</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>[9, 10, 13]</t>
+          <t>[9, 11, 12, 13]</t>
         </is>
       </c>
       <c r="H102" t="b">
@@ -4632,7 +4632,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.18|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.15|x7: 0.06|x8: 0.00|x9: 0.07|x10: 0.23|x11: 0.00|x12: 0.21|x13: 0.19|x14: 0.12|x15: 0.00|x16: 0.09|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.07|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.09|x7: 0.11|x8: 0.06|x9: 0.13|x10: 0.00|x11: 0.20|x12: 0.27|x13: 0.06|x14: 0.08|x15: 0.00|x16: 0.13|x17: 0.00</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -4642,12 +4642,12 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.23]</t>
+          <t>[0.00, 0.08, 0.27]</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>[10, 12]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H103" t="b">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.00|x4: 0.07|x5: 0.00|x6: 0.10|x7: 0.08|x8: 0.06|x9: 0.09|x10: 0.20|x11: 0.00|x12: 0.00|x13: 0.22|x14: 0.18|x15: 0.17|x16: 0.07|x17: 0.00</t>
+          <t>x1: 0.13|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.19|x7: 0.00|x8: 0.00|x9: 0.09|x10: 0.00|x11: 0.18|x12: 0.43|x13: 0.00|x14: 0.21|x15: 0.00|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -4683,19 +4683,19 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.22]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -4714,7 +4714,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.16|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.09|x8: 0.00|x9: 0.06|x10: 0.12|x11: 0.00|x12: 0.10|x13: 0.07|x14: 0.32|x15: 0.29|x16: 0.09|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.07|x10: 0.11|x11: 0.13|x12: 0.22|x13: 0.09|x14: 0.29|x15: 0.34|x16: 0.06|x17: 0.00</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -4724,12 +4724,12 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.32]</t>
+          <t>[0.00, 0.08, 0.34]</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>[14, 15]</t>
+          <t>[12, 14, 15]</t>
         </is>
       </c>
       <c r="H105" t="b">
@@ -4755,7 +4755,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.17|x3: 0.00|x4: 0.06|x5: 0.00|x6: 0.00|x7: 0.07|x8: 0.00|x9: 0.00|x10: 0.21|x11: 0.00|x12: 0.15|x13: 0.17|x14: 0.40|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.12|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.23|x12: 0.36|x13: 0.08|x14: 0.43|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -4765,12 +4765,12 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.40]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>[10, 14]</t>
+          <t>[11, 12, 14]</t>
         </is>
       </c>
       <c r="H106" t="b">
@@ -4796,7 +4796,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.23|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.15|x8: 0.00|x9: 0.11|x10: 0.21|x11: 0.00|x12: 0.25|x13: 0.25|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.15|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.27|x10: 0.00|x11: 0.10|x12: 0.21|x13: 0.00|x14: 0.26|x15: 0.19|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -4806,19 +4806,19 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.27]</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>[2, 10, 12, 13]</t>
+          <t>[9, 12, 14]</t>
         </is>
       </c>
       <c r="H107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -4837,7 +4837,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.11|x3: 0.13|x4: 0.00|x5: 0.00|x6: 0.11|x7: 0.00|x8: 0.00|x9: 0.14|x10: 0.23|x11: 0.00|x12: 0.13|x13: 0.31|x14: 0.14|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.11|x4: 0.00|x5: 0.00|x6: 0.12|x7: 0.00|x8: 0.07|x9: 0.15|x10: 0.00|x11: 0.13|x12: 0.30|x13: 0.09|x14: 0.21|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -4847,19 +4847,19 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.30]</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.10|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.06|x10: 0.28|x11: 0.00|x12: 0.07|x13: 0.26|x14: 0.31|x15: 0.07|x16: 0.09|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.14|x7: 0.00|x8: 0.00|x9: 0.10|x10: 0.00|x11: 0.11|x12: 0.27|x13: 0.18|x14: 0.29|x15: 0.07|x16: 0.06|x17: 0.00</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -4888,12 +4888,12 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.29]</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>[10, 13, 14]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H109" t="b">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.09|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.00|x9: 0.11|x10: 0.22|x11: 0.00|x12: 0.00|x13: 0.19|x14: 0.21|x15: 0.27|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.00|x9: 0.17|x10: 0.00|x11: 0.12|x12: 0.29|x13: 0.00|x14: 0.40|x15: 0.17|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -4929,12 +4929,12 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.40]</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>[10, 14, 15]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H110" t="b">
@@ -4960,7 +4960,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.00|x3: 0.10|x4: 0.07|x5: 0.00|x6: 0.11|x7: 0.00|x8: 0.00|x9: 0.09|x10: 0.21|x11: 0.00|x12: 0.09|x13: 0.23|x14: 0.06|x15: 0.17|x16: 0.10|x17: 0.00</t>
+          <t>x1: 0.17|x2: 0.00|x3: 0.13|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.14|x10: 0.00|x11: 0.15|x12: 0.27|x13: 0.10|x14: 0.18|x15: 0.16|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -4970,12 +4970,12 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.23]</t>
+          <t>[0.00, 0.08, 0.27]</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H111" t="b">
@@ -5001,7 +5001,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.36|x11: 0.00|x12: 0.14|x13: 0.39|x14: 0.07|x15: 0.26|x16: 0.07|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.06|x9: 0.00|x10: 0.00|x11: 0.28|x12: 0.43|x13: 0.17|x14: 0.06|x15: 0.20|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -5011,12 +5011,12 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.39]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>[10, 13, 15]</t>
+          <t>[11, 12, 15]</t>
         </is>
       </c>
       <c r="H112" t="b">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.11|x3: 0.11|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.19|x9: 0.08|x10: 0.26|x11: 0.00|x12: 0.15|x13: 0.24|x14: 0.00|x15: 0.11|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.00|x3: 0.09|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.16|x9: 0.11|x10: 0.08|x11: 0.13|x12: 0.23|x13: 0.12|x14: 0.15|x15: 0.07|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -5052,12 +5052,12 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.26]</t>
+          <t>[0.00, 0.08, 0.23]</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H113" t="b">
@@ -5083,7 +5083,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.06|x3: 0.06|x4: 0.08|x5: 0.00|x6: 0.21|x7: 0.00|x8: 0.00|x9: 0.15|x10: 0.18|x11: 0.00|x12: 0.08|x13: 0.18|x14: 0.00|x15: 0.22|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.22|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.13|x7: 0.00|x8: 0.06|x9: 0.17|x10: 0.00|x11: 0.13|x12: 0.26|x13: 0.00|x14: 0.13|x15: 0.20|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -5093,19 +5093,19 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.22]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>[6, 15]</t>
+          <t>[1, 12]</t>
         </is>
       </c>
       <c r="H114" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I114" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -5124,7 +5124,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.08|x3: 0.00|x4: 0.00|x5: 0.24|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.11|x10: 0.18|x11: 0.00|x12: 0.00|x13: 0.19|x14: 0.10|x15: 0.31|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.14|x5: 0.11|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.06|x11: 0.14|x12: 0.23|x13: 0.00|x14: 0.22|x15: 0.28|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -5134,12 +5134,12 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>[5, 15]</t>
+          <t>[12, 14, 15]</t>
         </is>
       </c>
       <c r="H115" t="b">
@@ -5165,7 +5165,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.10|x3: 0.14|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.13|x11: 0.00|x12: 0.08|x13: 0.20|x14: 0.13|x15: 0.28|x16: 0.15|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.16|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.17|x12: 0.32|x13: 0.10|x14: 0.15|x15: 0.25|x16: 0.09|x17: 0.00</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -5175,12 +5175,12 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.28]</t>
+          <t>[0.00, 0.08, 0.32]</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>[13, 15]</t>
+          <t>[12, 15]</t>
         </is>
       </c>
       <c r="H116" t="b">
@@ -5206,7 +5206,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.07|x9: 0.10|x10: 0.30|x11: 0.00|x12: 0.06|x13: 0.28|x14: 0.12|x15: 0.17|x16: 0.08|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.08|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.20|x12: 0.48|x13: 0.18|x14: 0.19|x15: 0.17|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -5216,12 +5216,12 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.30]</t>
+          <t>[0.00, 0.08, 0.48]</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H117" t="b">
@@ -5247,7 +5247,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.07|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.31|x11: 0.00|x12: 0.08|x13: 0.29|x14: 0.26|x15: 0.16|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.14|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.11|x9: 0.00|x10: 0.00|x11: 0.17|x12: 0.39|x13: 0.00|x14: 0.23|x15: 0.18|x16: 0.09|x17: 0.00</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -5257,12 +5257,12 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.39]</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>[10, 13, 14]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H118" t="b">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.06|x3: 0.00|x4: 0.11|x5: 0.00|x6: 0.12|x7: 0.07|x8: 0.00|x9: 0.16|x10: 0.16|x11: 0.00|x12: 0.00|x13: 0.16|x14: 0.08|x15: 0.30|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.17|x2: 0.05|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.06|x8: 0.00|x9: 0.14|x10: 0.00|x11: 0.13|x12: 0.31|x13: 0.06|x14: 0.06|x15: 0.17|x16: 0.06|x17: 0.00</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -5298,19 +5298,19 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.30]</t>
+          <t>[0.00, 0.08, 0.31]</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.14|x3: 0.15|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.25|x11: 0.00|x12: 0.17|x13: 0.21|x14: 0.07|x15: 0.13|x16: 0.18|x17: 0.00</t>
+          <t>x1: 0.19|x2: 0.00|x3: 0.15|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.09|x11: 0.18|x12: 0.34|x13: 0.00|x14: 0.13|x15: 0.16|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -5339,12 +5339,12 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.34]</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H120" t="b">
@@ -5370,7 +5370,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.11|x3: 0.11|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.14|x8: 0.06|x9: 0.00|x10: 0.19|x11: 0.11|x12: 0.24|x13: 0.29|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.00|x3: 0.16|x4: 0.00|x5: 0.00|x6: 0.11|x7: 0.00|x8: 0.07|x9: 0.09|x10: 0.00|x11: 0.19|x12: 0.34|x13: 0.07|x14: 0.05|x15: 0.00|x16: 0.12|x17: 0.00</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -5380,12 +5380,12 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.34]</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>[12, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H121" t="b">
@@ -5411,7 +5411,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.10|x3: 0.12|x4: 0.10|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.25|x11: 0.00|x12: 0.22|x13: 0.27|x14: 0.00|x15: 0.09|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.16|x2: 0.00|x3: 0.17|x4: 0.00|x5: 0.00|x6: 0.11|x7: 0.00|x8: 0.00|x9: 0.10|x10: 0.00|x11: 0.18|x12: 0.40|x13: 0.06|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -5421,12 +5421,12 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.40]</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>[10, 12, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H122" t="b">
@@ -5452,7 +5452,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>x1: 0.16|x2: 0.00|x3: 0.00|x4: 0.18|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.05|x10: 0.35|x11: 0.00|x12: 0.07|x13: 0.48|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.21|x2: 0.00|x3: 0.00|x4: 0.09|x5: 0.07|x6: 0.00|x7: 0.00|x8: 0.15|x9: 0.13|x10: 0.00|x11: 0.17|x12: 0.28|x13: 0.12|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -5462,12 +5462,12 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.48]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[1, 12]</t>
         </is>
       </c>
       <c r="H123" t="b">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>x1: 0.20|x2: 0.07|x3: 0.00|x4: 0.18|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.25|x11: 0.00|x12: 0.18|x13: 0.25|x14: 0.11|x15: 0.00|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.29|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.09|x7: 0.00|x8: 0.09|x9: 0.00|x10: 0.09|x11: 0.24|x12: 0.43|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -5503,12 +5503,12 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[1, 11, 12]</t>
         </is>
       </c>
       <c r="H124" t="b">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.15|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.13|x10: 0.26|x11: 0.00|x12: 0.20|x13: 0.51|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.16|x2: 0.00|x3: 0.00|x4: 0.07|x5: 0.08|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.13|x10: 0.00|x11: 0.21|x12: 0.49|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -5544,12 +5544,12 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.51]</t>
+          <t>[0.00, 0.08, 0.49]</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H125" t="b">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.10|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.27|x7: 0.05|x8: 0.00|x9: 0.00|x10: 0.33|x11: 0.00|x12: 0.09|x13: 0.35|x14: 0.00|x15: 0.00|x16: 0.11|x17: 0.00</t>
+          <t>x1: 0.28|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.12|x7: 0.00|x8: 0.10|x9: 0.07|x10: 0.06|x11: 0.16|x12: 0.38|x13: 0.00|x14: 0.12|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -5585,12 +5585,12 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.35]</t>
+          <t>[0.00, 0.08, 0.38]</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>[6, 10, 13]</t>
+          <t>[1, 12]</t>
         </is>
       </c>
       <c r="H126" t="b">
@@ -5616,7 +5616,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.13|x9: 0.21|x10: 0.21|x11: 0.00|x12: 0.12|x13: 0.49|x14: 0.14|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.06|x7: 0.00|x8: 0.19|x9: 0.16|x10: 0.00|x11: 0.19|x12: 0.22|x13: 0.26|x14: 0.15|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -5626,12 +5626,12 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.49]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>[9, 10, 13]</t>
+          <t>[12, 13]</t>
         </is>
       </c>
       <c r="H127" t="b">
@@ -5657,7 +5657,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.09|x3: 0.35|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.14|x8: 0.07|x9: 0.08|x10: 0.16|x11: 0.10|x12: 0.06|x13: 0.18|x14: 0.00|x15: 0.00|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.36|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.13|x9: 0.08|x10: 0.00|x11: 0.24|x12: 0.22|x13: 0.11|x14: 0.00|x15: 0.00|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -5667,12 +5667,12 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.35]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 11, 12]</t>
         </is>
       </c>
       <c r="H128" t="b">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.20|x3: 0.12|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.00|x9: 0.09|x10: 0.27|x11: 0.00|x12: 0.00|x13: 0.38|x14: 0.14|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.17|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.13|x10: 0.00|x11: 0.28|x12: 0.61|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -5708,12 +5708,12 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.38]</t>
+          <t>[0.00, 0.08, 0.61]</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H129" t="b">
@@ -5739,7 +5739,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.15|x3: 0.25|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.11|x10: 0.28|x11: 0.00|x12: 0.00|x13: 0.32|x14: 0.19|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.23|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.06|x10: 0.08|x11: 0.17|x12: 0.41|x13: 0.09|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -5749,12 +5749,12 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.32]</t>
+          <t>[0.00, 0.08, 0.41]</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>[3, 10, 13]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="H130" t="b">
@@ -5780,7 +5780,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.27|x4: 0.00|x5: 0.16|x6: 0.09|x7: 0.07|x8: 0.12|x9: 0.15|x10: 0.22|x11: 0.00|x12: 0.00|x13: 0.14|x14: 0.00|x15: 0.09|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.16|x2: 0.00|x3: 0.21|x4: 0.12|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.18|x10: 0.11|x11: 0.08|x12: 0.18|x13: 0.07|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -5790,12 +5790,12 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.21]</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>[3, 10]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="H131" t="b">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.43|x4: 0.00|x5: 0.21|x6: 0.08|x7: 0.00|x8: 0.10|x9: 0.00|x10: 0.21|x11: 0.00|x12: 0.00|x13: 0.19|x14: 0.00|x15: 0.08|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.43|x4: 0.16|x5: 0.15|x6: 0.00|x7: 0.00|x8: 0.08|x9: 0.00|x10: 0.00|x11: 0.07|x12: 0.17|x13: 0.00|x14: 0.07|x15: 0.00|x16: 0.09|x17: 0.00</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>[3, 5, 10]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="H132" t="b">
@@ -5862,7 +5862,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.07|x3: 0.13|x4: 0.10|x5: 0.00|x6: 0.06|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.22|x11: 0.00|x12: 0.00|x13: 0.29|x14: 0.34|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.18|x2: 0.00|x3: 0.16|x4: 0.12|x5: 0.09|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.17|x12: 0.35|x13: 0.00|x14: 0.25|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -5872,12 +5872,12 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.34]</t>
+          <t>[0.00, 0.08, 0.35]</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>[10, 13, 14]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H133" t="b">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.20|x3: 0.23|x4: 0.07|x5: 0.12|x6: 0.00|x7: 0.00|x8: 0.13|x9: 0.08|x10: 0.08|x11: 0.00|x12: 0.25|x13: 0.00|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.33|x4: 0.07|x5: 0.06|x6: 0.10|x7: 0.00|x8: 0.07|x9: 0.22|x10: 0.00|x11: 0.09|x12: 0.21|x13: 0.10|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -5913,12 +5913,12 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.33]</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>[3, 12]</t>
+          <t>[3, 9, 12]</t>
         </is>
       </c>
       <c r="H134" t="b">
@@ -5944,7 +5944,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.08|x3: 0.16|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.10|x10: 0.15|x11: 0.00|x12: 0.23|x13: 0.38|x14: 0.10|x15: 0.00|x16: 0.10|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.15|x4: 0.06|x5: 0.11|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.14|x10: 0.10|x11: 0.09|x12: 0.19|x13: 0.00|x14: 0.06|x15: 0.00|x16: 0.18|x17: 0.00</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -5954,12 +5954,12 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.38]</t>
+          <t>[0.00, 0.08, 0.19]</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>[12, 13]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H135" t="b">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.10|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.11|x9: 0.19|x10: 0.29|x11: 0.00|x12: 0.00|x13: 0.34|x14: 0.06|x15: 0.00|x16: 0.05|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.13|x9: 0.18|x10: 0.07|x11: 0.23|x12: 0.37|x13: 0.23|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -5995,19 +5995,19 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.34]</t>
+          <t>[0.00, 0.08, 0.37]</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12, 13]</t>
         </is>
       </c>
       <c r="H136" t="b">
         <v>0</v>
       </c>
       <c r="I136" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -6026,7 +6026,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.14|x3: 0.00|x4: 0.10|x5: 0.25|x6: 0.00|x7: 0.00|x8: 0.11|x9: 0.12|x10: 0.15|x11: 0.00|x12: 0.11|x13: 0.15|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.16|x2: 0.00|x3: 0.00|x4: 0.21|x5: 0.16|x6: 0.00|x7: 0.00|x8: 0.15|x9: 0.20|x10: 0.00|x11: 0.10|x12: 0.25|x13: 0.07|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -6041,14 +6041,14 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>[5]</t>
+          <t>[4, 9, 12]</t>
         </is>
       </c>
       <c r="H137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -6067,7 +6067,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>x1: 0.15|x2: 0.16|x3: 0.07|x4: 0.19|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.00|x10: 0.10|x11: 0.06|x12: 0.11|x13: 0.08|x14: 0.18|x15: 0.11|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.21|x5: 0.17|x6: 0.00|x7: 0.00|x8: 0.16|x9: 0.06|x10: 0.08|x11: 0.11|x12: 0.15|x13: 0.00|x14: 0.36|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -6077,19 +6077,19 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.19]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[4, 14]</t>
         </is>
       </c>
       <c r="H138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -6108,7 +6108,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.16|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.00|x9: 0.10|x10: 0.32|x11: 0.00|x12: 0.05|x13: 0.50|x14: 0.11|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.06|x3: 0.00|x4: 0.09|x5: 0.07|x6: 0.00|x7: 0.07|x8: 0.08|x9: 0.09|x10: 0.00|x11: 0.15|x12: 0.35|x13: 0.09|x14: 0.16|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -6118,12 +6118,12 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.50]</t>
+          <t>[0.00, 0.08, 0.35]</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H139" t="b">
@@ -6149,7 +6149,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.21|x7: 0.11|x8: 0.08|x9: 0.00|x10: 0.14|x11: 0.05|x12: 0.05|x13: 0.21|x14: 0.13|x15: 0.24|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.14|x7: 0.13|x8: 0.07|x9: 0.00|x10: 0.00|x11: 0.21|x12: 0.13|x13: 0.20|x14: 0.15|x15: 0.21|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -6159,19 +6159,19 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.24]</t>
+          <t>[0.00, 0.08, 0.21]</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>[6, 13, 15]</t>
+          <t>[11, 15]</t>
         </is>
       </c>
       <c r="H140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -6190,7 +6190,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.38|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.06|x8: 0.00|x9: 0.00|x10: 0.16|x11: 0.00|x12: 0.00|x13: 0.21|x14: 0.31|x15: 0.11|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.11|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.17|x9: 0.43|x10: 0.05|x11: 0.13|x12: 0.24|x13: 0.16|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -6200,12 +6200,12 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.38]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>[2, 13, 14]</t>
+          <t>[9, 12]</t>
         </is>
       </c>
       <c r="H141" t="b">
@@ -6231,7 +6231,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.16|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.13|x10: 0.31|x11: 0.00|x12: 0.08|x13: 0.32|x14: 0.00|x15: 0.00|x16: 0.19|x17: 0.00</t>
+          <t>x1: 0.14|x2: 0.00|x3: 0.00|x4: 0.08|x5: 0.12|x6: 0.00|x7: 0.00|x8: 0.13|x9: 0.08|x10: 0.13|x11: 0.13|x12: 0.31|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.17|x17: 0.00</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -6241,12 +6241,12 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.32]</t>
+          <t>[0.00, 0.08, 0.31]</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H142" t="b">
@@ -6272,7 +6272,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.18|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.08|x9: 0.08|x10: 0.21|x11: 0.06|x12: 0.16|x13: 0.27|x14: 0.09|x15: 0.06|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.14|x9: 0.20|x10: 0.00|x11: 0.23|x12: 0.37|x13: 0.11|x14: 0.17|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -6282,12 +6282,12 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.37]</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[9, 11, 12]</t>
         </is>
       </c>
       <c r="H143" t="b">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.13|x3: 0.08|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.14|x8: 0.16|x9: 0.21|x10: 0.10|x11: 0.00|x12: 0.00|x13: 0.19|x14: 0.16|x15: 0.14|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.06|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.09|x8: 0.35|x9: 0.23|x10: 0.00|x11: 0.13|x12: 0.17|x13: 0.12|x14: 0.00|x15: 0.00|x16: 0.07|x17: 0.00</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -6323,19 +6323,19 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.21]</t>
+          <t>[0.00, 0.08, 0.35]</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[8, 9]</t>
         </is>
       </c>
       <c r="H144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -6354,7 +6354,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.12|x3: 0.00|x4: 0.06|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.19|x9: 0.15|x10: 0.18|x11: 0.00|x12: 0.18|x13: 0.31|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.21|x9: 0.20|x10: 0.00|x11: 0.20|x12: 0.40|x13: 0.12|x14: 0.00|x15: 0.08|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -6364,19 +6364,19 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.40]</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[8, 11, 12]</t>
         </is>
       </c>
       <c r="H145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.09|x3: 0.00|x4: 0.06|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.33|x9: 0.06|x10: 0.27|x11: 0.00|x12: 0.00|x13: 0.27|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.11|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.34|x9: 0.22|x10: 0.00|x11: 0.16|x12: 0.22|x13: 0.16|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -6405,12 +6405,12 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.33]</t>
+          <t>[0.00, 0.08, 0.34]</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>[8, 10, 13]</t>
+          <t>[8, 9, 12]</t>
         </is>
       </c>
       <c r="H146" t="b">
@@ -6436,7 +6436,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.13|x3: 0.00|x4: 0.00|x5: 0.07|x6: 0.00|x7: 0.11|x8: 0.00|x9: 0.34|x10: 0.18|x11: 0.00|x12: 0.26|x13: 0.21|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.19|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.08|x9: 0.36|x10: 0.00|x11: 0.18|x12: 0.39|x13: 0.11|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -6446,12 +6446,12 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.34]</t>
+          <t>[0.00, 0.08, 0.39]</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>[9, 12, 13]</t>
+          <t>[9, 12]</t>
         </is>
       </c>
       <c r="H147" t="b">
@@ -6477,7 +6477,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.07|x3: 0.10|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.22|x8: 0.00|x9: 0.00|x10: 0.22|x11: 0.23|x12: 0.00|x13: 0.40|x14: 0.06|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.10|x8: 0.13|x9: 0.18|x10: 0.00|x11: 0.32|x12: 0.37|x13: 0.20|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -6487,12 +6487,12 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.40]</t>
+          <t>[0.00, 0.08, 0.37]</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>[7, 10, 11, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H148" t="b">
@@ -6518,7 +6518,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>x1: 0.20|x2: 0.12|x3: 0.06|x4: 0.19|x5: 0.22|x6: 0.00|x7: 0.07|x8: 0.07|x9: 0.00|x10: 0.21|x11: 0.00|x12: 0.00|x13: 0.11|x14: 0.00|x15: 0.00|x16: 0.06|x17: 0.00</t>
+          <t>x1: 0.36|x2: 0.00|x3: 0.06|x4: 0.11|x5: 0.09|x6: 0.00|x7: 0.06|x8: 0.00|x9: 0.06|x10: 0.00|x11: 0.21|x12: 0.27|x13: 0.08|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -6528,19 +6528,19 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.22]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>[5, 10]</t>
+          <t>[1, 11, 12]</t>
         </is>
       </c>
       <c r="H149" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I149" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -6559,7 +6559,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>x1: 0.09|x2: 0.19|x3: 0.00|x4: 0.11|x5: 0.11|x6: 0.00|x7: 0.00|x8: 0.08|x9: 0.00|x10: 0.11|x11: 0.00|x12: 0.29|x13: 0.24|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.00|x3: 0.00|x4: 0.08|x5: 0.06|x6: 0.07|x7: 0.00|x8: 0.10|x9: 0.06|x10: 0.00|x11: 0.19|x12: 0.45|x13: 0.10|x14: 0.10|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -6569,12 +6569,12 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.45]</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>[12, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H150" t="b">
@@ -6600,7 +6600,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.13|x3: 0.14|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.08|x9: 0.16|x10: 0.29|x11: 0.00|x12: 0.00|x13: 0.26|x14: 0.09|x15: 0.00|x16: 0.09|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.18|x4: 0.08|x5: 0.07|x6: 0.00|x7: 0.00|x8: 0.18|x9: 0.00|x10: 0.00|x11: 0.26|x12: 0.53|x13: 0.00|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -6610,19 +6610,19 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.53]</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H151" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I151" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -6641,7 +6641,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.11|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.29|x8: 0.00|x9: 0.19|x10: 0.14|x11: 0.26|x12: 0.08|x13: 0.14|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.05|x9: 0.00|x10: 0.00|x11: 0.47|x12: 0.47|x13: 0.20|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -6651,12 +6651,12 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.29]</t>
+          <t>[0.00, 0.08, 0.47]</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>[7, 11]</t>
+          <t>[11, 12]</t>
         </is>
       </c>
       <c r="H152" t="b">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.25|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.23|x7: 0.06|x8: 0.00|x9: 0.16|x10: 0.18|x11: 0.00|x12: 0.11|x13: 0.11|x14: 0.20|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.21|x7: 0.00|x8: 0.10|x9: 0.36|x10: 0.00|x11: 0.13|x12: 0.24|x13: 0.10|x14: 0.08|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -6692,12 +6692,12 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.36]</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>[2, 6]</t>
+          <t>[6, 9, 12]</t>
         </is>
       </c>
       <c r="H153" t="b">
@@ -6723,7 +6723,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>x1: 0.10|x2: 0.00|x3: 0.00|x4: 0.13|x5: 0.06|x6: 0.12|x7: 0.00|x8: 0.07|x9: 0.08|x10: 0.23|x11: 0.00|x12: 0.08|x13: 0.25|x14: 0.07|x15: 0.12|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.15|x7: 0.00|x8: 0.14|x9: 0.06|x10: 0.00|x11: 0.20|x12: 0.43|x13: 0.00|x14: 0.09|x15: 0.12|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -6733,12 +6733,12 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.43]</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H154" t="b">
@@ -6764,7 +6764,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>x1: 0.12|x2: 0.13|x3: 0.00|x4: 0.13|x5: 0.06|x6: 0.00|x7: 0.00|x8: 0.13|x9: 0.14|x10: 0.18|x11: 0.00|x12: 0.16|x13: 0.17|x14: 0.07|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.08|x5: 0.11|x6: 0.00|x7: 0.00|x8: 0.15|x9: 0.08|x10: 0.05|x11: 0.19|x12: 0.32|x13: 0.08|x14: 0.00|x15: 0.00|x16: 0.12|x17: 0.00</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -6774,19 +6774,19 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.18]</t>
+          <t>[0.00, 0.08, 0.32]</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H155" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I155" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
@@ -6805,7 +6805,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>x1: 0.08|x2: 0.08|x3: 0.09|x4: 0.06|x5: 0.08|x6: 0.00|x7: 0.00|x8: 0.10|x9: 0.07|x10: 0.27|x11: 0.00|x12: 0.12|x13: 0.35|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.06|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.11|x9: 0.08|x10: 0.00|x11: 0.18|x12: 0.44|x13: 0.00|x14: 0.23|x15: 0.00|x16: 0.08|x17: 0.00</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -6815,19 +6815,19 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.35]</t>
+          <t>[0.00, 0.08, 0.44]</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="H156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -6846,7 +6846,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.12|x10: 0.18|x11: 0.00|x12: 0.10|x13: 0.25|x14: 0.28|x15: 0.36|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.08|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.19|x12: 0.32|x13: 0.00|x14: 0.41|x15: 0.31|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -6856,12 +6856,12 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.41]</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>[13, 14, 15]</t>
+          <t>[12, 14, 15]</t>
         </is>
       </c>
       <c r="H157" t="b">
@@ -6887,7 +6887,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.09|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.11|x8: 0.08|x9: 0.18|x10: 0.11|x11: 0.06|x12: 0.08|x13: 0.23|x14: 0.36|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.07|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.07|x7: 0.00|x8: 0.11|x9: 0.13|x10: 0.00|x11: 0.12|x12: 0.17|x13: 0.23|x14: 0.22|x15: 0.19|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -6897,7 +6897,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.36]</t>
+          <t>[0.00, 0.08, 0.23]</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -6928,7 +6928,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.12|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.18|x7: 0.12|x8: 0.15|x9: 0.15|x10: 0.13|x11: 0.00|x12: 0.11|x13: 0.15|x14: 0.19|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.13|x7: 0.00|x8: 0.12|x9: 0.23|x10: 0.00|x11: 0.16|x12: 0.19|x13: 0.06|x14: 0.34|x15: 0.07|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -6938,19 +6938,19 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.19]</t>
+          <t>[0.00, 0.08, 0.34]</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[9, 14]</t>
         </is>
       </c>
       <c r="H159" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I159" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -6969,7 +6969,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.19|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.06|x7: 0.00|x8: 0.00|x9: 0.14|x10: 0.16|x11: 0.00|x12: 0.15|x13: 0.27|x14: 0.11|x15: 0.14|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.08|x2: 0.10|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.09|x7: 0.13|x8: 0.06|x9: 0.11|x10: 0.00|x11: 0.16|x12: 0.22|x13: 0.07|x14: 0.11|x15: 0.18|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -6979,12 +6979,12 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.27]</t>
+          <t>[0.00, 0.08, 0.22]</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H160" t="b">
@@ -7010,7 +7010,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>x1: 0.06|x2: 0.00|x3: 0.00|x4: 0.07|x5: 0.00|x6: 0.00|x7: 0.06|x8: 0.07|x9: 0.00|x10: 0.18|x11: 0.00|x12: 0.05|x13: 0.26|x14: 0.00|x15: 0.54|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.15|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.00|x11: 0.16|x12: 0.37|x13: 0.11|x14: 0.14|x15: 0.37|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -7020,12 +7020,12 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.54]</t>
+          <t>[0.00, 0.08, 0.37]</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>[13, 15]</t>
+          <t>[12, 15]</t>
         </is>
       </c>
       <c r="H161" t="b">
@@ -7051,7 +7051,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.08|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.00|x7: 0.00|x8: 0.14|x9: 0.11|x10: 0.23|x11: 0.00|x12: 0.18|x13: 0.24|x14: 0.08|x15: 0.17|x16: 0.07|x17: 0.00</t>
+          <t>x1: 0.06|x2: 0.00|x3: 0.12|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.15|x9: 0.00|x10: 0.00|x11: 0.18|x12: 0.34|x13: 0.09|x14: 0.10|x15: 0.10|x16: 0.10|x17: 0.00</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -7061,12 +7061,12 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.24]</t>
+          <t>[0.00, 0.08, 0.34]</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H162" t="b">
@@ -7092,7 +7092,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>x1: 0.09|x2: 0.00|x3: 0.11|x4: 0.00|x5: 0.00|x6: 0.08|x7: 0.00|x8: 0.00|x9: 0.00|x10: 0.35|x11: 0.06|x12: 0.13|x13: 0.29|x14: 0.00|x15: 0.00|x16: 0.19|x17: 0.00</t>
+          <t>x1: 0.09|x2: 0.00|x3: 0.07|x4: 0.00|x5: 0.11|x6: 0.00|x7: 0.00|x8: 0.05|x9: 0.00|x10: 0.12|x11: 0.17|x12: 0.24|x13: 0.06|x14: 0.11|x15: 0.00|x16: 0.29|x17: 0.00</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -7102,19 +7102,19 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.35]</t>
+          <t>[0.00, 0.08, 0.29]</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[12, 16]</t>
         </is>
       </c>
       <c r="H163" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I163" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -7133,7 +7133,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>x1: 0.07|x2: 0.00|x3: 0.08|x4: 0.10|x5: 0.08|x6: 0.00|x7: 0.00|x8: 0.09|x9: 0.00|x10: 0.28|x11: 0.00|x12: 0.09|x13: 0.31|x14: 0.06|x15: 0.00|x16: 0.13|x17: 0.00</t>
+          <t>x1: 0.12|x2: 0.00|x3: 0.00|x4: 0.14|x5: 0.20|x6: 0.00|x7: 0.00|x8: 0.08|x9: 0.00|x10: 0.00|x11: 0.12|x12: 0.22|x13: 0.06|x14: 0.09|x15: 0.00|x16: 0.26|x17: 0.00</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -7143,19 +7143,19 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.31]</t>
+          <t>[0.00, 0.08, 0.26]</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>[10, 13]</t>
+          <t>[5, 12, 16]</t>
         </is>
       </c>
       <c r="H164" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I164" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -7174,7 +7174,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>x1: 0.00|x2: 0.13|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.10|x7: 0.21|x8: 0.13|x9: 0.00|x10: 0.24|x11: 0.14|x12: 0.09|x13: 0.25|x14: 0.00|x15: 0.00|x16: 0.00|x17: 0.00</t>
+          <t>x1: 0.00|x2: 0.00|x3: 0.00|x4: 0.00|x5: 0.00|x6: 0.05|x7: 0.07|x8: 0.19|x9: 0.22|x10: 0.00|x11: 0.28|x12: 0.27|x13: 0.12|x14: 0.09|x15: 0.00|x16: 0.00|x17: 0.00</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -7184,12 +7184,12 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>[0.00, 0.08, 0.25]</t>
+          <t>[0.00, 0.08, 0.28]</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>[7, 10, 13]</t>
+          <t>[9, 11, 12]</t>
         </is>
       </c>
       <c r="H165" t="b">

</xml_diff>